<commit_message>
Fix typo in Triple Crown races excel doc.
</commit_message>
<xml_diff>
--- a/triplecrown/out/20180611/ttt_races.xlsx
+++ b/triplecrown/out/20180611/ttt_races.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vyee/Projects/other/running-ds/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vyee/Projects/other/running-ds/triplecrown/out/20180611/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30580" yWindow="-20020" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="12800" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="races" sheetId="2" r:id="rId1"/>
@@ -286,7 +286,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Belmon Stakes
+      <t xml:space="preserve">Belmont Stakes
 </t>
     </r>
     <r>
@@ -446,277 +446,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
-        <color theme="1"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="h:mm:ss.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
         <color rgb="FF000000"/>
         <name val="Roboto Mono"/>
         <scheme val="none"/>
@@ -759,25 +488,6 @@
         <name val="Roboto Mono"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="h:mm:ss.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <name val="Roboto Mono"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
@@ -853,6 +563,296 @@
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="h:mm:ss.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Mono"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -864,19 +864,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A2:D5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A2:D5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <tableColumns count="4">
-    <tableColumn id="1" name="Column1" headerRowDxfId="0" dataDxfId="9"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="1" dataDxfId="8"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="2" dataDxfId="7"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="3" dataDxfId="6"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="20" dataDxfId="19"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="18" dataDxfId="17"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="16" dataDxfId="15"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="14" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K29" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K29" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:K29">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -891,19 +891,19 @@
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" name="place" dataDxfId="13"/>
-    <tableColumn id="2" name="name" dataDxfId="12"/>
-    <tableColumn id="3" name="city" dataDxfId="10"/>
-    <tableColumn id="4" name="gender" dataDxfId="11"/>
-    <tableColumn id="5" name="age" dataDxfId="22"/>
-    <tableColumn id="6" name="division" dataDxfId="21">
+    <tableColumn id="1" name="place" dataDxfId="10"/>
+    <tableColumn id="2" name="name" dataDxfId="9"/>
+    <tableColumn id="3" name="city" dataDxfId="8"/>
+    <tableColumn id="4" name="gender" dataDxfId="7"/>
+    <tableColumn id="5" name="age" dataDxfId="6"/>
+    <tableColumn id="6" name="division" dataDxfId="5">
       <calculatedColumnFormula>IF(AND(D2="M",E2&lt;50),"Men &lt;50",IF(AND(D2="M",E2&gt;=50),"Men 50+",IF(AND(D2="F",E2&lt;50),"Women &lt;50","Women 50+")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="pos_ttt" dataDxfId="20"/>
-    <tableColumn id="8" name="time_ttt" dataDxfId="19"/>
-    <tableColumn id="9" name="pos_lctc" dataDxfId="18"/>
-    <tableColumn id="10" name="time_lctc" dataDxfId="17"/>
-    <tableColumn id="11" name="time_total" dataDxfId="16"/>
+    <tableColumn id="7" name="pos_ttt" dataDxfId="4"/>
+    <tableColumn id="8" name="time_ttt" dataDxfId="3"/>
+    <tableColumn id="9" name="pos_lctc" dataDxfId="2"/>
+    <tableColumn id="10" name="time_lctc" dataDxfId="1"/>
+    <tableColumn id="11" name="time_total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1174,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1263,16 +1263,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="2" max="2" width="26.5" style="5" customWidth="1"/>
+    <col min="3" max="3" width="21" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.83203125" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" customWidth="1"/>

</xml_diff>